<commit_message>
Update programmer 's task_list
</commit_message>
<xml_diff>
--- a/Docs/cahier de doléances.xlsx
+++ b/Docs/cahier de doléances.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Unity\3D\Erebos\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Erebos\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" tabRatio="266" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270" tabRatio="266" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="_internal" sheetId="7" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Todo - LD" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Todo!$A$1:$D$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Todo!$A$1:$D$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Todo - GD'!$A$1:$D$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Todo - LD'!$A$1:$D$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Todo - LD'!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Notes</t>
   </si>
@@ -70,19 +70,7 @@
     <t>collectibles qui manque d'intérêt</t>
   </si>
   <si>
-    <t>rajouter 2nd plume dans la Z2</t>
-  </si>
-  <si>
-    <t>signe eclatos</t>
-  </si>
-  <si>
-    <t>remonter death fog Z1 &amp; Z2</t>
-  </si>
-  <si>
     <t>reverse move sing Z2</t>
-  </si>
-  <si>
-    <t>bug  "woody wood pecker"</t>
   </si>
   <si>
     <t>death en movable sing =&gt; gros bug</t>
@@ -94,15 +82,6 @@
     <t>looper les musiques</t>
   </si>
   <si>
-    <t>avancer Cp après la ptit colline</t>
-  </si>
-  <si>
-    <t>une sorte de flèche pour indiquer le sense de lecture</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (genre vers les collectibles)</t>
-  </si>
-  <si>
     <t>3eme sing move à monter un peu plus</t>
   </si>
   <si>
@@ -112,88 +91,13 @@
     <t>ptet 1 T de trop Z2</t>
   </si>
   <si>
-    <t>premier eclatos du jeu, en blanc éclaté</t>
-  </si>
-  <si>
-    <t>mettre piQUES 3eme collectibles</t>
-  </si>
-  <si>
-    <t>nemesis ajouter CP</t>
-  </si>
-  <si>
-    <t>LD</t>
-  </si>
-  <si>
     <t>Z1</t>
-  </si>
-  <si>
-    <t>Z1 / Z2</t>
-  </si>
-  <si>
-    <t>Z2</t>
   </si>
   <si>
     <t>reverse movable sing</t>
   </si>
   <si>
     <t>video splash screen</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>slerp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> black sing au lieu d'un RotateTowards</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>implemener</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> head quand on est dans un</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> black hole</t>
-    </r>
   </si>
   <si>
     <r>
@@ -231,88 +135,6 @@
       </rPr>
       <t>éclatos</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">indiquer qu'une </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>manette</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> est fortement </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>conseillée</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">implementatiion des </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sons</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de Matthieu GD</t>
-    </r>
-  </si>
-  <si>
-    <t>options language dans un dropdown</t>
-  </si>
-  <si>
-    <t>dropdown fléchées</t>
-  </si>
-  <si>
-    <t>voir concept art UI</t>
   </si>
 </sst>
 </file>
@@ -473,121 +295,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="92">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="0"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="80">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1682,11 +1390,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1:D9"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,7 +1423,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1724,45 +1432,35 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="7" t="s">
-        <v>39</v>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="1"/>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -1784,22 +1482,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1810,32 +1500,20 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2054,42 +1732,36 @@
       <c r="C51" s="1"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="3"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:D12">
-    <sortCondition ref="C2:C12" customList="Urgent,High,Medium,Low,Very Low"/>
+  <sortState ref="A3:D7">
+    <sortCondition ref="C3:C7" customList="Urgent,High,Medium,Low,Very Low"/>
   </sortState>
-  <conditionalFormatting sqref="C24:C49 D21:D23 A18:C23 A1:D17 D18:D19">
-    <cfRule type="containsText" dxfId="91" priority="47" operator="containsText" text="Urgent">
+  <conditionalFormatting sqref="C23:C48 D20:D22 A17:C22 D17:D18 A1:D16">
+    <cfRule type="containsText" dxfId="79" priority="47" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="50" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="78" priority="50" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="51" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="77" priority="51" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="53" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="76" priority="53" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",D20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",D20)))</formula>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",D19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",D19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",D19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",D19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2101,7 +1773,7 @@
           <x14:formula1>
             <xm:f>_internal!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C17 C18:C49</xm:sqref>
+          <xm:sqref>C2:C48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2154,7 +1826,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -2481,58 +2153,58 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D22:D24 A1:D1 A25:D25 C26:C53 D13:D20 A13:C24 A4:D12">
-    <cfRule type="containsText" dxfId="83" priority="21" operator="containsText" text="Urgent">
+    <cfRule type="containsText" dxfId="71" priority="21" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="22" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="70" priority="22" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="23" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="69" priority="23" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="24" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="68" priority="24" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="79" priority="17" operator="containsText" text="Urgent">
+    <cfRule type="containsText" dxfId="67" priority="17" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="18" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="66" priority="18" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="19" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="65" priority="19" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",D21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="20" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="64" priority="20" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",D21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D2">
-    <cfRule type="containsText" dxfId="75" priority="13" operator="containsText" text="Urgent">
+    <cfRule type="containsText" dxfId="63" priority="13" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="14" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="62" priority="14" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="15" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="61" priority="15" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="16" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="60" priority="16" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:D3">
-    <cfRule type="containsText" dxfId="71" priority="9" operator="containsText" text="Urgent">
+    <cfRule type="containsText" dxfId="59" priority="9" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="10" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="58" priority="10" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="11" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="57" priority="11" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="12" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="56" priority="12" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2555,11 +2227,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2586,64 +2258,62 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>32</v>
-      </c>
+      <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="1"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -2655,92 +2325,50 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="1"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2763,37 +2391,37 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="1"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="1"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="1"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="7"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="7"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="1"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="7"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1"/>
       <c r="D25" s="3"/>
     </row>
@@ -3061,319 +2689,216 @@
       <c r="C69" s="1"/>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="3"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:D16">
-    <sortCondition ref="C2:C16" customList="Urgent,High,Medium,Low,Very Low"/>
+  <sortState ref="A2:D9">
+    <sortCondition ref="C2:C9" customList="Urgent,High,Medium,Low,Very Low"/>
   </sortState>
-  <conditionalFormatting sqref="D30:D35 A17:C35 D17:D28 C36:C69 A1:D1 A4:A6">
-    <cfRule type="containsText" dxfId="67" priority="65" operator="containsText" text="Urgent">
+  <conditionalFormatting sqref="D27:D32 A14:C32 D14:D25 C33:C66 A1:D1 A2:A3">
+    <cfRule type="containsText" dxfId="55" priority="65" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="66" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="54" priority="66" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="67" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="53" priority="67" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="52" priority="68" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="containsText" dxfId="63" priority="61" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",D29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="62" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",D29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="63" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",D29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="64" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",D29)))</formula>
+  <conditionalFormatting sqref="D26">
+    <cfRule type="containsText" dxfId="51" priority="61" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",D26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="50" priority="62" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",D26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="49" priority="63" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",D26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="48" priority="64" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",D26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D3">
-    <cfRule type="containsText" dxfId="59" priority="53" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="54" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="56" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",A3)))</formula>
+  <conditionalFormatting sqref="B2:D2">
+    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="46" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="47" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="48" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:D4">
-    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",B4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="50" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",B4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="51" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",B4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="52" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",B4)))</formula>
+  <conditionalFormatting sqref="B3:D3">
+    <cfRule type="containsText" dxfId="43" priority="41" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:D5">
-    <cfRule type="containsText" dxfId="51" priority="45" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",B5)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="48" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",B5)))</formula>
+  <conditionalFormatting sqref="A4:D4">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",A4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",A4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="39" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",A4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:D6">
-    <cfRule type="containsText" dxfId="47" priority="41" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="42" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="43" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",B6)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="44" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",B6)))</formula>
+  <conditionalFormatting sqref="A5:D5">
+    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",A5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",A5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",A5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",A5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:D7">
-    <cfRule type="containsText" dxfId="43" priority="37" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",A7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="38" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",A7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="39" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",A7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="40" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",A7)))</formula>
+  <conditionalFormatting sqref="A6:D6">
+    <cfRule type="containsText" dxfId="31" priority="29" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",A6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="30" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",A6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="31" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",A6)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",A6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:D8">
-    <cfRule type="containsText" dxfId="39" priority="33" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",A8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",A8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",A8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",A8)))</formula>
+  <conditionalFormatting sqref="C7">
+    <cfRule type="containsText" dxfId="27" priority="25" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",C7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="26" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",C7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="27" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",C7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A9:D9">
-    <cfRule type="containsText" dxfId="35" priority="29" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",A9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="30" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",A9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",A9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",A9)))</formula>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="23" priority="21" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="22" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="23" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",C9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",C9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="Urgent">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="28" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="containsText" dxfId="27" priority="21" operator="containsText" text="Urgent">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="23" priority="17" operator="containsText" text="Urgent">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Urgent">
       <formula>NOT(ISERROR(SEARCH("Urgent",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="18" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="Medium">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Medium">
       <formula>NOT(ISERROR(SEARCH("Medium",C12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="High">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="High">
       <formula>NOT(ISERROR(SEARCH("High",C12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",C13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",C13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",C13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",C14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",C14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C14)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",C14)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",C15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",C15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",C15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",C15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A16:D16">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Urgent">
-      <formula>NOT(ISERROR(SEARCH("Urgent",A16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",A16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",A16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",A16)))</formula>
+  <conditionalFormatting sqref="A13:D13">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Urgent">
+      <formula>NOT(ISERROR(SEARCH("Urgent",A13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",A13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Medium">
+      <formula>NOT(ISERROR(SEARCH("Medium",A13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="High">
+      <formula>NOT(ISERROR(SEARCH("High",A13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="57" operator="containsText" text="Urgent" id="{78FDDF6D-58F3-49B2-91CC-6F0BEC531024}">
-            <xm:f>NOT(ISERROR(SEARCH("Urgent",Todo!A2)))</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <fgColor theme="0"/>
-                  <bgColor rgb="FFFF0000"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="58" operator="containsText" text="Low" id="{CF0500AA-F284-48D3-B490-8C5037ADF3DC}">
-            <xm:f>NOT(ISERROR(SEARCH("Low",Todo!A2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="59" operator="containsText" text="Medium" id="{4EC3CA00-3276-4920-8212-99D0984DD964}">
-            <xm:f>NOT(ISERROR(SEARCH("Medium",Todo!A2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C6500"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFEB9C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="60" operator="containsText" text="High" id="{ED0A6E26-7696-4902-9D29-21F0FFFABD2D}">
-            <xm:f>NOT(ISERROR(SEARCH("High",Todo!A2)))</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A2:D2</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>_internal!$B$1:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C69</xm:sqref>
+          <xm:sqref>C2:C66</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Respawn collectibles if player die with collectible
</commit_message>
<xml_diff>
--- a/Docs/cahier de doléances.xlsx
+++ b/Docs/cahier de doléances.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270" tabRatio="266" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="12270" tabRatio="266" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="_internal" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>Notes</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>plus de rewqard pour les tuto feather</t>
-  </si>
-  <si>
-    <t>looper les musiques</t>
   </si>
   <si>
     <t>3eme sing move à monter un peu plus</t>
@@ -1392,7 +1389,7 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="A2:D7"/>
     </sheetView>
@@ -1433,7 +1430,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -1443,7 +1440,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -2229,9 +2226,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="A6:C6"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,18 +2256,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -2279,10 +2272,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -2307,10 +2300,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>

</xml_diff>